<commit_message>
refactor: add changes to exception handling
</commit_message>
<xml_diff>
--- a/Config - SAP.xlsx
+++ b/Config - SAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatoradz\Documents\UiPath\SAP General Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038D795D-52F3-4132-8A89-D2E0CF3FA8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E93143-8099-4CDA-9C86-64F63740CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,18 +216,6 @@
     <t>Folder Path to store completed data</t>
   </si>
   <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\Template Folder</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\Original Folder</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\Completed Folder</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\Error Screenshot Folder</t>
-  </si>
-  <si>
     <t>1800000</t>
   </si>
   <si>
@@ -281,6 +269,18 @@
   </si>
   <si>
     <t>VA02</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\00 Template</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\01 Original</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\02 Completed</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\03 Error Screenshot</t>
   </si>
 </sst>
 </file>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF062F7A-1854-46C6-9CB6-57934E58DB32}">
   <dimension ref="A1:Z1032"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -908,7 +908,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>42</v>
@@ -922,7 +922,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>40</v>
@@ -934,13 +934,13 @@
         <v>16</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -962,10 +962,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>35</v>
@@ -976,7 +976,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>47</v>
@@ -1016,7 +1016,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>22</v>
@@ -1028,7 +1028,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>43</v>
@@ -1039,24 +1039,24 @@
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="C19" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>70</v>
-      </c>
       <c r="C20" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
@@ -1064,7 +1064,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>57</v>
@@ -1075,7 +1075,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C22" s="29" t="s">
         <v>55</v>
@@ -1087,7 +1087,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>58</v>
@@ -1098,7 +1098,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
feat: add some revision in process
</commit_message>
<xml_diff>
--- a/Config - SAP.xlsx
+++ b/Config - SAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatoradz\Documents\UiPath\SAP General Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E93143-8099-4CDA-9C86-64F63740CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E46D2A-7A75-4916-9DD2-5DD0A1F4BED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,16 +271,16 @@
     <t>VA02</t>
   </si>
   <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\00 Template</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\01 Original</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\02 Completed</t>
-  </si>
-  <si>
-    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\ID - Data Process SCOM (SO Reject)\03 Error Screenshot</t>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\SAP General Framework\00 Template</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\SAP General Framework\01 Original</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\SAP General Framework\02 Completed</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\Documents\Dzikri\Projects\SAP General Framework\03 Error Screenshot</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:Z1032"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat: add file error handler
</commit_message>
<xml_diff>
--- a/Config - SAP.xlsx
+++ b/Config - SAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://danone-my.sharepoint.com/personal/dzikri_hatorangan_external_danone_com/Documents/Documents/UiPath/SAP General Framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{50E46D2A-7A75-4916-9DD2-5DD0A1F4BED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{471D628E-DB44-4E64-BD6E-DB491501B3C1}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{50E46D2A-7A75-4916-9DD2-5DD0A1F4BED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535E955B-1CEC-4277-931E-8C3A58BAA239}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>SAP_Username</t>
   </si>
   <si>
-    <t>SAP_Password</t>
-  </si>
-  <si>
     <t>IDRBT02Q-RPA</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
   </si>
   <si>
     <t>SAP Logon SAP Username</t>
-  </si>
-  <si>
-    <t>SAP Logon SAP Password</t>
   </si>
   <si>
     <t>Email for Unexpected Error</t>
@@ -278,6 +272,15 @@
   </si>
   <si>
     <t>C:\Users\hatoradz\Documents\Dzikri\Projects\SAP General Framework\03 Error Screenshot</t>
+  </si>
+  <si>
+    <t>Process Folder</t>
+  </si>
+  <si>
+    <t>Folder path for processing files</t>
+  </si>
+  <si>
+    <t>C:\Users\hatoradz\OneDrive - Danone\Documents\Dzikri\Projects\SAP General Framework\04 Process</t>
   </si>
 </sst>
 </file>
@@ -762,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF062F7A-1854-46C6-9CB6-57934E58DB32}">
-  <dimension ref="A1:Z1032"/>
+  <dimension ref="A1:Z1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -789,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -846,7 +849,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -858,7 +861,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="11"/>
     </row>
@@ -891,212 +894,212 @@
         <v>31</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="C9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>49</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>71</v>
+      <c r="A10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="C15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:26" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="22"/>
+        <v>21</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>60</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>64</v>
+    <row r="20" spans="1:4" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:4" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="31" t="s">
-        <v>57</v>
+      <c r="C22" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="28" t="s">
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="30"/>
-    </row>
-    <row r="23" spans="1:4" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
+      <c r="C23" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>58</v>
-      </c>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="D24" s="11"/>
     </row>
@@ -1119,43 +1122,43 @@
     <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="46" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="181" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="181" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="50" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="51" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="52" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="53" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="137.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="137.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="60" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="117.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="117.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="68" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="69" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="70" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="28.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="28.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="74" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="77" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1178,8 +1181,8 @@
     <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1196,9 +1199,9 @@
     <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2104,7 +2107,6 @@
     <row r="1029" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1030" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1031" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1032" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2116,7 +2118,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2164,13 +2166,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>